<commit_message>
Connect backend operation and frontend visualization. Optimization process works
</commit_message>
<xml_diff>
--- a/code/flask-server/Database esami_Ing_Ind_Inf.xlsx
+++ b/code/flask-server/Database esami_Ing_Ind_Inf.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\SchedulEx\code\flask-server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopet\OneDrive\Documents\0.POLIMI\Magistrale\6. SoftwareEngineering\Schedulex\code\flask-server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED66A73-288B-492C-8E4D-1086CD1ABD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAC270A-E0A1-49D6-9B64-2F742B034A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ATM" sheetId="1" r:id="rId1"/>
     <sheet name="ELT" sheetId="2" r:id="rId2"/>
-    <sheet name="Foglio3" sheetId="4" r:id="rId3"/>
+    <sheet name="total" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="66">
   <si>
     <t>ATM</t>
   </si>
@@ -1088,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1337,286 +1337,19 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>88692</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6">
-        <v>176</v>
-      </c>
-      <c r="M6">
-        <v>5</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <v>29</v>
-      </c>
+      <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>85744</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7">
-        <v>176</v>
-      </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7">
-        <v>10</v>
-      </c>
-      <c r="O7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="2">
-        <v>82740</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="2">
-        <v>176</v>
-      </c>
-      <c r="M8" s="2">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2">
-        <v>10</v>
-      </c>
-      <c r="O8" s="2">
-        <v>29</v>
-      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>88691</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>3</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9">
-        <v>176</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
-      <c r="N9">
-        <v>10</v>
-      </c>
-      <c r="O9">
-        <v>29</v>
-      </c>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>82748</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10">
-        <v>176</v>
-      </c>
-      <c r="M10">
-        <v>5</v>
-      </c>
-      <c r="N10">
-        <v>10</v>
-      </c>
-      <c r="O10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>85796</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>2</v>
-      </c>
-      <c r="G11">
-        <v>4</v>
-      </c>
-      <c r="H11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11">
-        <v>176</v>
-      </c>
-      <c r="M11">
-        <v>5</v>
-      </c>
-      <c r="N11">
-        <v>10</v>
-      </c>
-      <c r="O11">
-        <v>29</v>
-      </c>
+      <c r="J10" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
@@ -1626,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AFBC0AA-A1B3-4B37-BE0B-1AAFB0090F24}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,50 +1464,50 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3">
+        <v>85746</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
-        <v>82740</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="2">
+      <c r="H3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3">
         <v>176</v>
       </c>
-      <c r="M3" s="2">
-        <v>5</v>
-      </c>
-      <c r="N3" s="2">
-        <v>10</v>
-      </c>
-      <c r="O3" s="2">
+      <c r="M3">
+        <v>5</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
         <v>29</v>
       </c>
     </row>
@@ -1783,31 +1516,31 @@
         <v>64</v>
       </c>
       <c r="B4">
-        <v>85742</v>
+        <v>85754</v>
       </c>
       <c r="C4" t="s">
         <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
       <c r="G4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="K4" t="s">
         <v>27</v>
@@ -1822,335 +1555,6 @@
         <v>10</v>
       </c>
       <c r="O4">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5">
-        <v>93279</v>
-      </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>3</v>
-      </c>
-      <c r="H5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5">
-        <v>176</v>
-      </c>
-      <c r="M5">
-        <v>5</v>
-      </c>
-      <c r="N5">
-        <v>10</v>
-      </c>
-      <c r="O5">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6">
-        <v>88694</v>
-      </c>
-      <c r="C6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6">
-        <v>176</v>
-      </c>
-      <c r="M6">
-        <v>5</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7">
-        <v>82741</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>20</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" t="s">
-        <v>44</v>
-      </c>
-      <c r="L7">
-        <v>176</v>
-      </c>
-      <c r="M7">
-        <v>5</v>
-      </c>
-      <c r="N7">
-        <v>10</v>
-      </c>
-      <c r="O7">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8">
-        <v>82747</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8">
-        <v>176</v>
-      </c>
-      <c r="M8">
-        <v>5</v>
-      </c>
-      <c r="N8">
-        <v>10</v>
-      </c>
-      <c r="O8">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B9">
-        <v>52348</v>
-      </c>
-      <c r="C9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>2</v>
-      </c>
-      <c r="I9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K9" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9">
-        <v>176</v>
-      </c>
-      <c r="M9">
-        <v>5</v>
-      </c>
-      <c r="N9">
-        <v>10</v>
-      </c>
-      <c r="O9">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10">
-        <v>85746</v>
-      </c>
-      <c r="C10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <v>4</v>
-      </c>
-      <c r="H10" t="s">
-        <v>2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" t="s">
-        <v>27</v>
-      </c>
-      <c r="L10">
-        <v>176</v>
-      </c>
-      <c r="M10">
-        <v>5</v>
-      </c>
-      <c r="N10">
-        <v>10</v>
-      </c>
-      <c r="O10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11">
-        <v>85754</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11">
-        <v>3</v>
-      </c>
-      <c r="G11">
-        <v>6</v>
-      </c>
-      <c r="H11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L11">
-        <v>176</v>
-      </c>
-      <c r="M11">
-        <v>5</v>
-      </c>
-      <c r="N11">
-        <v>10</v>
-      </c>
-      <c r="O11">
         <v>29</v>
       </c>
     </row>
@@ -2163,15 +1567,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87202A33-6A29-492F-9873-CBFE207FC65B}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="20.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C1" t="s">
@@ -2218,7 +1628,7 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>88697</v>
       </c>
       <c r="C2" t="s">
@@ -2265,7 +1675,7 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="3">
         <v>82746</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -2312,7 +1722,7 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>85743</v>
       </c>
       <c r="C4" t="s">
@@ -2359,7 +1769,7 @@
       <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>85745</v>
       </c>
       <c r="C5" t="s">
@@ -2406,7 +1816,7 @@
       <c r="A6" t="s">
         <v>0</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>88692</v>
       </c>
       <c r="C6" t="s">
@@ -2453,7 +1863,7 @@
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>85744</v>
       </c>
       <c r="C7" t="s">
@@ -2500,7 +1910,7 @@
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>82740</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -2547,7 +1957,7 @@
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>88691</v>
       </c>
       <c r="C9" t="s">
@@ -2594,7 +2004,7 @@
       <c r="A10" t="s">
         <v>0</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>82748</v>
       </c>
       <c r="C10" t="s">
@@ -2641,7 +2051,7 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>85796</v>
       </c>
       <c r="C11" t="s">
@@ -2688,7 +2098,7 @@
       <c r="A12" t="s">
         <v>64</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>85742</v>
       </c>
       <c r="C12" t="s">
@@ -2735,7 +2145,7 @@
       <c r="A13" t="s">
         <v>64</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>93279</v>
       </c>
       <c r="C13" t="s">
@@ -2782,7 +2192,7 @@
       <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>88694</v>
       </c>
       <c r="C14" t="s">
@@ -2829,7 +2239,7 @@
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>82741</v>
       </c>
       <c r="C15" t="s">
@@ -2876,7 +2286,7 @@
       <c r="A16" t="s">
         <v>64</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>82747</v>
       </c>
       <c r="C16" t="s">
@@ -2923,7 +2333,7 @@
       <c r="A17" t="s">
         <v>64</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>52348</v>
       </c>
       <c r="C17" t="s">
@@ -2970,7 +2380,7 @@
       <c r="A18" t="s">
         <v>64</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>85746</v>
       </c>
       <c r="C18" t="s">
@@ -3017,7 +2427,7 @@
       <c r="A19" t="s">
         <v>64</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>85754</v>
       </c>
       <c r="C19" t="s">

</xml_diff>